<commit_message>
fix: generaba la cantidad de archivos json son cantidad de filas incluyendo todas la filas en todos los archivos, ademas de fallos en la conversion de campos nulos a null
</commit_message>
<xml_diff>
--- a/archivos_excel/ccfPlantilla.xlsx
+++ b/archivos_excel/ccfPlantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AT-RedAbierta\Documents\Local Repos\GoProcesadorExcel\archivos_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1660CD-264B-491A-9F8A-21D6E9870F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F888BED5-D3EA-4230-8B3E-E0AEB0D0D907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="125">
   <si>
     <t>CodigoCondicionOperacion</t>
   </si>
@@ -382,6 +382,39 @@
   </si>
   <si>
     <t>Valor10</t>
+  </si>
+  <si>
+    <t>COMISION POR RECEPCION DE 0 PAGOS RECIBIDOS EN EL MES DE DICIEMBRE 2033</t>
+  </si>
+  <si>
+    <t>COMISION POR RECEPCION DE 0 PAGOS RECIBIDOS EN EL MES DE DICIEMBRE 2034</t>
+  </si>
+  <si>
+    <t>Campo11</t>
+  </si>
+  <si>
+    <t>Etiqueta11</t>
+  </si>
+  <si>
+    <t>Valor11</t>
+  </si>
+  <si>
+    <t>Campo12</t>
+  </si>
+  <si>
+    <t>Etiqueta12</t>
+  </si>
+  <si>
+    <t>Valor12</t>
+  </si>
+  <si>
+    <t>Campo13</t>
+  </si>
+  <si>
+    <t>Etiqueta13</t>
+  </si>
+  <si>
+    <t>Valor13</t>
   </si>
 </sst>
 </file>
@@ -2235,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7BA81E-3122-44E4-BC7E-16857C584094}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="A3:O11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2693,7 +2726,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2732,6 +2765,94 @@
         <v>0</v>
       </c>
       <c r="N11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>99</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>114</v>
+      </c>
+      <c r="J12">
+        <v>20</v>
+      </c>
+      <c r="K12">
+        <v>15</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>99</v>
+      </c>
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>115</v>
+      </c>
+      <c r="J13">
+        <v>20</v>
+      </c>
+      <c r="K13">
+        <v>15</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
         <v>15</v>
       </c>
     </row>
@@ -2743,10 +2864,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC022B76-0322-4241-B913-68E820CF55C5}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2905,6 +3026,48 @@
         <v>113</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>